<commit_message>
Add more info to the popup.
</commit_message>
<xml_diff>
--- a/president.xlsx
+++ b/president.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="120" windowWidth="33580" windowHeight="20300" tabRatio="500"/>
+    <workbookView xWindow="220" yWindow="220" windowWidth="33340" windowHeight="20080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Presidnets" sheetId="2" r:id="rId1"/>
@@ -49,6 +49,471 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="257">
   <si>
+    <t>September 19, 1881 - March 4, 1885</t>
+  </si>
+  <si>
+    <t>March 4, 1885 - March 4, 1889, March 4, 1893 - March 4, 1897</t>
+  </si>
+  <si>
+    <t>March 4, 1889 - March 4, 1893</t>
+  </si>
+  <si>
+    <t>March 4, 1897 - September 14, 1901</t>
+  </si>
+  <si>
+    <t>September 14, 1901 - March 4, 1909</t>
+  </si>
+  <si>
+    <t>March 4, 1909 - March 4, 1913</t>
+  </si>
+  <si>
+    <t>March 4, 1913 - March 4, 1921</t>
+  </si>
+  <si>
+    <t>March 4, 1921 - August 2, 1923</t>
+  </si>
+  <si>
+    <t>August 2, 1923 - March 4, 1929</t>
+  </si>
+  <si>
+    <t>March 4, 1929 - March 4, 1933</t>
+  </si>
+  <si>
+    <t>March 4, 1933 - April 12, 1945</t>
+  </si>
+  <si>
+    <t>April 12, 1945 - January 20, 1953</t>
+  </si>
+  <si>
+    <t>January 20, 1953 - January 20, 1961</t>
+  </si>
+  <si>
+    <t>January 20, 1961 - November 22, 1963</t>
+  </si>
+  <si>
+    <t>November 22, 1963 - January 20, 1969</t>
+  </si>
+  <si>
+    <t>January 20, 1969 - August 9, 1974</t>
+  </si>
+  <si>
+    <t>August 9, 1974 - January 20, 1977</t>
+  </si>
+  <si>
+    <t>January 20, 1977 - January 20, 1981</t>
+  </si>
+  <si>
+    <t>January 20, 1981 - January 20, 1989</t>
+  </si>
+  <si>
+    <t>January 20, 1989 - January 20, 1993</t>
+  </si>
+  <si>
+    <t>January 20, 1993 - January 20, 2001</t>
+  </si>
+  <si>
+    <t>January 20, 2001 - January 20, 2009</t>
+  </si>
+  <si>
+    <t>November 2, 1795</t>
+  </si>
+  <si>
+    <t>Pineville</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>January 7, 1800</t>
+  </si>
+  <si>
+    <t>Summerhill</t>
+  </si>
+  <si>
+    <t>November 23, 1804</t>
+  </si>
+  <si>
+    <t>Hillsborough</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>December 29, 1808</t>
+  </si>
+  <si>
+    <t>Raleigh</t>
+  </si>
+  <si>
+    <t>Dwight D. Eisenhower</t>
+  </si>
+  <si>
+    <t>John F. Kennedy</t>
+  </si>
+  <si>
+    <t>Lyndon B. Johnson</t>
+  </si>
+  <si>
+    <t>Jimmy Carter</t>
+  </si>
+  <si>
+    <t>Ronald Reagan</t>
+  </si>
+  <si>
+    <t>George H. W. Bush</t>
+  </si>
+  <si>
+    <t>Bill Clinton</t>
+  </si>
+  <si>
+    <t>George W. Bush</t>
+  </si>
+  <si>
+    <t>William McKinley</t>
+  </si>
+  <si>
+    <t>Theodore Roosevelt</t>
+  </si>
+  <si>
+    <t>William Howard Taft</t>
+  </si>
+  <si>
+    <t>Woodrow Wilson</t>
+  </si>
+  <si>
+    <t>Warren G. Harding</t>
+  </si>
+  <si>
+    <t>Calvin Coolidge</t>
+  </si>
+  <si>
+    <t>Herbert Hoover</t>
+  </si>
+  <si>
+    <t>Franklin D. Roosevelt</t>
+  </si>
+  <si>
+    <t>Harry S. Truman</t>
+  </si>
+  <si>
+    <t>Andrew Johnson</t>
+  </si>
+  <si>
+    <t>Ulysses S. Grant</t>
+  </si>
+  <si>
+    <t>Rutherford B. Hayes</t>
+  </si>
+  <si>
+    <t>James A. Garfield</t>
+  </si>
+  <si>
+    <t>Chester A. Arthur</t>
+  </si>
+  <si>
+    <t>Grover Cleveland</t>
+  </si>
+  <si>
+    <t>Benjamin Harrison</t>
+  </si>
+  <si>
+    <t>Martin Van Buren</t>
+  </si>
+  <si>
+    <t>William Henry Harrison</t>
+  </si>
+  <si>
+    <t>John Tyler</t>
+  </si>
+  <si>
+    <t>James K. Polk</t>
+  </si>
+  <si>
+    <t>Zachary Taylor</t>
+  </si>
+  <si>
+    <t>Millard Fillmore</t>
+  </si>
+  <si>
+    <t>Franklin Pierce</t>
+  </si>
+  <si>
+    <t>James Buchanan</t>
+  </si>
+  <si>
+    <t>Abraham Lincoln</t>
+  </si>
+  <si>
+    <t>President</t>
+  </si>
+  <si>
+    <t>George Washington</t>
+  </si>
+  <si>
+    <t>John Adams</t>
+  </si>
+  <si>
+    <t>Federalist</t>
+  </si>
+  <si>
+    <t>Thomas Jefferson</t>
+  </si>
+  <si>
+    <t>James Madison</t>
+  </si>
+  <si>
+    <t>James Monroe</t>
+  </si>
+  <si>
+    <t>John Quincy Adams</t>
+  </si>
+  <si>
+    <t>Andrew Jackson</t>
+  </si>
+  <si>
+    <t>April 30, 1789 - March 4, 1797</t>
+  </si>
+  <si>
+    <t>March 4, 1797 - March 4, 1801</t>
+  </si>
+  <si>
+    <t>March 4, 1801 - March 4, 1809</t>
+  </si>
+  <si>
+    <t>March 4, 1809 - March 4, 1817</t>
+  </si>
+  <si>
+    <t>March 4, 1817 - March 4, 1825</t>
+  </si>
+  <si>
+    <t>March 4, 1825 - March 4, 1829</t>
+  </si>
+  <si>
+    <t>March 4, 1829 - March 4, 1837</t>
+  </si>
+  <si>
+    <t>March 4, 1837 - March 4, 1841</t>
+  </si>
+  <si>
+    <t>March 4, 1841 - April 4, 1841</t>
+  </si>
+  <si>
+    <t>April 4, 1841 - March 4, 1845</t>
+  </si>
+  <si>
+    <t>March 4, 1845 - March 4, 1849</t>
+  </si>
+  <si>
+    <t>March 4, 1849 - July 9, 1850</t>
+  </si>
+  <si>
+    <t>July 9, 1850 - March 4, 1853</t>
+  </si>
+  <si>
+    <t>March 4, 1853 - March 4, 1857</t>
+  </si>
+  <si>
+    <t>March 4, 1857 - March 4, 1861</t>
+  </si>
+  <si>
+    <t>March 4, 1861 - April 15, 1865</t>
+  </si>
+  <si>
+    <t>April 15, 1865 - March 4, 1869</t>
+  </si>
+  <si>
+    <t>March 4, 1869 - March 4, 1877</t>
+  </si>
+  <si>
+    <t>March 4, 1877 - March 4, 1881</t>
+  </si>
+  <si>
+    <t>March 4, 1881 - September 19, 1881</t>
+  </si>
+  <si>
+    <t>August 20, 1833</t>
+  </si>
+  <si>
+    <t>North Bend</t>
+  </si>
+  <si>
+    <t>March 18, 1837</t>
+  </si>
+  <si>
+    <t>Caldwell</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>January 29, 1843</t>
+  </si>
+  <si>
+    <t>Niles</t>
+  </si>
+  <si>
+    <t>December 28, 1856</t>
+  </si>
+  <si>
+    <t>Staunton</t>
+  </si>
+  <si>
+    <t>September 15, 1857</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>October 27, 1858</t>
+  </si>
+  <si>
+    <t>New York City</t>
+  </si>
+  <si>
+    <t>November 2, 1865</t>
+  </si>
+  <si>
+    <t>Blooming Grove</t>
+  </si>
+  <si>
+    <t>July 4, 1872</t>
+  </si>
+  <si>
+    <t>Plymouth</t>
+  </si>
+  <si>
+    <t>August 10, 1874</t>
+  </si>
+  <si>
+    <t>West Branch</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>January 30, 1882</t>
+  </si>
+  <si>
+    <t>Hyde Park</t>
+  </si>
+  <si>
+    <t>May 8, 1884</t>
+  </si>
+  <si>
+    <t>Lamar</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>October 14, 1890</t>
+  </si>
+  <si>
+    <t>Denison</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Brookline</t>
+  </si>
+  <si>
+    <t>Stonewall</t>
+  </si>
+  <si>
+    <t>Barack Obama</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>Birthplace</t>
+  </si>
+  <si>
+    <t>In office</t>
+  </si>
+  <si>
+    <t>February 22, 1732</t>
+  </si>
+  <si>
+    <t>Westmoreland County</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>October 30, 1735</t>
+  </si>
+  <si>
+    <t>Braintree</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>April 13, 1743</t>
+  </si>
+  <si>
+    <t>Shadwell</t>
+  </si>
+  <si>
+    <t>March 16, 1751</t>
+  </si>
+  <si>
+    <t>Port Conway</t>
+  </si>
+  <si>
+    <t>April 28, 1758</t>
+  </si>
+  <si>
+    <t>Monroe Hall</t>
+  </si>
+  <si>
+    <t>March 15, 1767</t>
+  </si>
+  <si>
+    <t>Waxhaws Region</t>
+  </si>
+  <si>
+    <t>South/North Carolina</t>
+  </si>
+  <si>
+    <t>July 11, 1767</t>
+  </si>
+  <si>
+    <t>February 9, 1773</t>
+  </si>
+  <si>
+    <t>Charles City County</t>
+  </si>
+  <si>
+    <t>December 5, 1782</t>
+  </si>
+  <si>
+    <t>Kinderhook</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>November 24, 1784</t>
+  </si>
+  <si>
+    <t>Barboursville</t>
+  </si>
+  <si>
+    <t>March 29, 1790</t>
+  </si>
+  <si>
+    <t>April 23, 1791</t>
+  </si>
+  <si>
+    <t>Cove Gap</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
     <t>lat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -231,18 +696,12 @@
     <t>WY</t>
   </si>
   <si>
-    <t>November 22, 1963 – January 20, 1969</t>
-  </si>
-  <si>
     <t>Tampico</t>
   </si>
   <si>
     <t>Illinois</t>
   </si>
   <si>
-    <t>January 20, 1981 – January 20, 1989</t>
-  </si>
-  <si>
     <t>Richard M. Nixon</t>
   </si>
   <si>
@@ -252,9 +711,6 @@
     <t>California</t>
   </si>
   <si>
-    <t>January 20, 1969 – August 9, 1974</t>
-  </si>
-  <si>
     <t>Gerald R. Ford</t>
   </si>
   <si>
@@ -264,50 +720,31 @@
     <t>Nebraska</t>
   </si>
   <si>
-    <t>August 9, 1974 – January 20, 1977</t>
-  </si>
-  <si>
     <t>Milton</t>
   </si>
   <si>
-    <t>January 20, 1989 – January 20, 1993</t>
-  </si>
-  <si>
     <t>Plains</t>
   </si>
   <si>
     <t>Georgia</t>
   </si>
   <si>
-    <t>January 20, 1977 – January 20, 1981</t>
-  </si>
-  <si>
     <t>New Haven</t>
   </si>
   <si>
     <t>Connecticut</t>
   </si>
   <si>
-    <t>January 20, 2001 – January 20, 2009</t>
-  </si>
-  <si>
     <t>Hope</t>
   </si>
   <si>
     <t>Arkansas</t>
   </si>
   <si>
-    <t>January 20, 1993 – January 20, 2001</t>
-  </si>
-  <si>
     <t>Honolulu</t>
   </si>
   <si>
     <t>Hawaii</t>
-  </si>
-  <si>
-    <t>March 4, 1885 – March 4, 1889, March 4, 1893 – March 4, 1897</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>January 20, 2009 - Present</t>
@@ -358,9 +795,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>April 15, 1865 – March 4, 1869</t>
-  </si>
-  <si>
     <t>February 12, 1809</t>
   </si>
   <si>
@@ -370,9 +804,6 @@
     <t>Kentucky</t>
   </si>
   <si>
-    <t>March 4, 1861 – April 15, 1865</t>
-  </si>
-  <si>
     <t>April 27, 1822</t>
   </si>
   <si>
@@ -382,18 +813,12 @@
     <t>Ohio</t>
   </si>
   <si>
-    <t>March 4, 1869 – March 4, 1877</t>
-  </si>
-  <si>
     <t>October 4, 1822</t>
   </si>
   <si>
     <t>Delaware</t>
   </si>
   <si>
-    <t>March 4, 1877 – March 4, 1881</t>
-  </si>
-  <si>
     <t>October 5, 1829</t>
   </si>
   <si>
@@ -403,447 +828,17 @@
     <t>Vermont</t>
   </si>
   <si>
-    <t>September 19, 1881 – March 4, 1885</t>
-  </si>
-  <si>
     <t>November 19, 1831</t>
   </si>
   <si>
     <t>Moreland Hills</t>
-  </si>
-  <si>
-    <t>March 4, 1881 – September 19, 1881</t>
-  </si>
-  <si>
-    <t>August 20, 1833</t>
-  </si>
-  <si>
-    <t>North Bend</t>
-  </si>
-  <si>
-    <t>March 4, 1889 – March 4, 1893</t>
-  </si>
-  <si>
-    <t>March 18, 1837</t>
-  </si>
-  <si>
-    <t>Caldwell</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>January 29, 1843</t>
-  </si>
-  <si>
-    <t>Niles</t>
-  </si>
-  <si>
-    <t>March 4, 1897 – September 14, 1901</t>
-  </si>
-  <si>
-    <t>December 28, 1856</t>
-  </si>
-  <si>
-    <t>Staunton</t>
-  </si>
-  <si>
-    <t>March 4, 1913 – March 4, 1921</t>
-  </si>
-  <si>
-    <t>September 15, 1857</t>
-  </si>
-  <si>
-    <t>Cincinnati</t>
-  </si>
-  <si>
-    <t>March 4, 1909 – March 4, 1913</t>
-  </si>
-  <si>
-    <t>October 27, 1858</t>
-  </si>
-  <si>
-    <t>New York City</t>
-  </si>
-  <si>
-    <t>September 14, 1901 – March 4, 1909</t>
-  </si>
-  <si>
-    <t>November 2, 1865</t>
-  </si>
-  <si>
-    <t>Blooming Grove</t>
-  </si>
-  <si>
-    <t>March 4, 1921 – August 2, 1923</t>
-  </si>
-  <si>
-    <t>July 4, 1872</t>
-  </si>
-  <si>
-    <t>Plymouth</t>
-  </si>
-  <si>
-    <t>August 2, 1923 – March 4, 1929</t>
-  </si>
-  <si>
-    <t>August 10, 1874</t>
-  </si>
-  <si>
-    <t>West Branch</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>March 4, 1929 – March 4, 1933</t>
-  </si>
-  <si>
-    <t>January 30, 1882</t>
-  </si>
-  <si>
-    <t>Hyde Park</t>
-  </si>
-  <si>
-    <t>March 4, 1933 – April 12, 1945</t>
-  </si>
-  <si>
-    <t>May 8, 1884</t>
-  </si>
-  <si>
-    <t>Lamar</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>April 12, 1945 – January 20, 1953</t>
-  </si>
-  <si>
-    <t>October 14, 1890</t>
-  </si>
-  <si>
-    <t>Denison</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>January 20, 1953 – January 20, 1961</t>
-  </si>
-  <si>
-    <t>Brookline</t>
-  </si>
-  <si>
-    <t>January 20, 1961 – November 22, 1963</t>
-  </si>
-  <si>
-    <t>Stonewall</t>
-  </si>
-  <si>
-    <t>Barack Obama</t>
-  </si>
-  <si>
-    <t>Date of birth</t>
-  </si>
-  <si>
-    <t>Birthplace</t>
-  </si>
-  <si>
-    <t>In office</t>
-  </si>
-  <si>
-    <t>February 22, 1732</t>
-  </si>
-  <si>
-    <t>Westmoreland County</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>April 30, 1789 – March 4, 1797</t>
-  </si>
-  <si>
-    <t>October 30, 1735</t>
-  </si>
-  <si>
-    <t>Braintree</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>March 4, 1797 – March 4, 1801</t>
-  </si>
-  <si>
-    <t>April 13, 1743</t>
-  </si>
-  <si>
-    <t>Shadwell</t>
-  </si>
-  <si>
-    <t>March 4, 1801 – March 4, 1809</t>
-  </si>
-  <si>
-    <t>March 16, 1751</t>
-  </si>
-  <si>
-    <t>Port Conway</t>
-  </si>
-  <si>
-    <t>March 4, 1809 – March 4, 1817</t>
-  </si>
-  <si>
-    <t>April 28, 1758</t>
-  </si>
-  <si>
-    <t>Monroe Hall</t>
-  </si>
-  <si>
-    <t>March 4, 1817 – March 4, 1825</t>
-  </si>
-  <si>
-    <t>March 15, 1767</t>
-  </si>
-  <si>
-    <t>Waxhaws Region</t>
-  </si>
-  <si>
-    <t>South/North Carolina</t>
-  </si>
-  <si>
-    <t>March 4, 1829 – March 4, 1837</t>
-  </si>
-  <si>
-    <t>July 11, 1767</t>
-  </si>
-  <si>
-    <t>March 4, 1825 – March 4, 1829</t>
-  </si>
-  <si>
-    <t>February 9, 1773</t>
-  </si>
-  <si>
-    <t>Charles City County</t>
-  </si>
-  <si>
-    <t>March 4, 1841 – April 4, 1841</t>
-  </si>
-  <si>
-    <t>December 5, 1782</t>
-  </si>
-  <si>
-    <t>Kinderhook</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>March 4, 1837 – March 4, 1841</t>
-  </si>
-  <si>
-    <t>November 24, 1784</t>
-  </si>
-  <si>
-    <t>Barboursville</t>
-  </si>
-  <si>
-    <t>March 4, 1849 – July 9, 1850</t>
-  </si>
-  <si>
-    <t>March 29, 1790</t>
-  </si>
-  <si>
-    <t>April 4, 1841 – March 4, 1845</t>
-  </si>
-  <si>
-    <t>April 23, 1791</t>
-  </si>
-  <si>
-    <t>Cove Gap</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>March 4, 1857 – March 4, 1861</t>
-  </si>
-  <si>
-    <t>November 2, 1795</t>
-  </si>
-  <si>
-    <t>Pineville</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>March 4, 1845 – March 4, 1849</t>
-  </si>
-  <si>
-    <t>January 7, 1800</t>
-  </si>
-  <si>
-    <t>Summerhill</t>
-  </si>
-  <si>
-    <t>July 9, 1850 – March 4, 1853</t>
-  </si>
-  <si>
-    <t>November 23, 1804</t>
-  </si>
-  <si>
-    <t>Hillsborough</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
-    <t>March 4, 1853 – March 4, 1857</t>
-  </si>
-  <si>
-    <t>December 29, 1808</t>
-  </si>
-  <si>
-    <t>Raleigh</t>
-  </si>
-  <si>
-    <t>Dwight D. Eisenhower</t>
-  </si>
-  <si>
-    <t>John F. Kennedy</t>
-  </si>
-  <si>
-    <t>Lyndon B. Johnson</t>
-  </si>
-  <si>
-    <t>Jimmy Carter</t>
-  </si>
-  <si>
-    <t>Ronald Reagan</t>
-  </si>
-  <si>
-    <t>George H. W. Bush</t>
-  </si>
-  <si>
-    <t>Bill Clinton</t>
-  </si>
-  <si>
-    <t>George W. Bush</t>
-  </si>
-  <si>
-    <t>William McKinley</t>
-  </si>
-  <si>
-    <t>Theodore Roosevelt</t>
-  </si>
-  <si>
-    <t>William Howard Taft</t>
-  </si>
-  <si>
-    <t>Woodrow Wilson</t>
-  </si>
-  <si>
-    <t>Warren G. Harding</t>
-  </si>
-  <si>
-    <t>Calvin Coolidge</t>
-  </si>
-  <si>
-    <t>Herbert Hoover</t>
-  </si>
-  <si>
-    <t>Franklin D. Roosevelt</t>
-  </si>
-  <si>
-    <t>Harry S. Truman</t>
-  </si>
-  <si>
-    <t>Andrew Johnson</t>
-  </si>
-  <si>
-    <t>Ulysses S. Grant</t>
-  </si>
-  <si>
-    <t>Rutherford B. Hayes</t>
-  </si>
-  <si>
-    <t>James A. Garfield</t>
-  </si>
-  <si>
-    <t>Chester A. Arthur</t>
-  </si>
-  <si>
-    <t>Grover Cleveland</t>
-  </si>
-  <si>
-    <t>Benjamin Harrison</t>
-  </si>
-  <si>
-    <t>Martin Van Buren</t>
-  </si>
-  <si>
-    <t>William Henry Harrison</t>
-  </si>
-  <si>
-    <t>John Tyler</t>
-  </si>
-  <si>
-    <t>James K. Polk</t>
-  </si>
-  <si>
-    <t>Zachary Taylor</t>
-  </si>
-  <si>
-    <t>Millard Fillmore</t>
-  </si>
-  <si>
-    <t>Franklin Pierce</t>
-  </si>
-  <si>
-    <t>James Buchanan</t>
-  </si>
-  <si>
-    <t>Abraham Lincoln</t>
-  </si>
-  <si>
-    <t>President</t>
-  </si>
-  <si>
-    <t>George Washington</t>
-  </si>
-  <si>
-    <t>John Adams</t>
-  </si>
-  <si>
-    <t>Federalist</t>
-  </si>
-  <si>
-    <t>Thomas Jefferson</t>
-  </si>
-  <si>
-    <t>James Madison</t>
-  </si>
-  <si>
-    <t>James Monroe</t>
-  </si>
-  <si>
-    <t>John Quincy Adams</t>
-  </si>
-  <si>
-    <t>Andrew Jackson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
@@ -1231,7 +1226,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I44"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1241,8 +1236,8 @@
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -1250,31 +1245,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>92</v>
+        <v>238</v>
       </c>
       <c r="B1" t="s">
-        <v>248</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>243</v>
       </c>
       <c r="F1" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="G1" t="s">
-        <v>87</v>
+        <v>233</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="I1" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1282,22 +1277,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>66</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F2" t="s">
-        <v>166</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>234</v>
       </c>
       <c r="H2">
         <v>38.186110999999997</v>
@@ -1311,22 +1306,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
-        <v>251</v>
+        <v>68</v>
       </c>
       <c r="H3">
         <v>42.239294000000001</v>
@@ -1340,22 +1335,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>69</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F4" t="s">
-        <v>173</v>
+        <v>76</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>235</v>
       </c>
       <c r="H4">
         <v>38.012383</v>
@@ -1369,22 +1364,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>253</v>
+        <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F5" t="s">
-        <v>176</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>235</v>
       </c>
       <c r="H5">
         <v>38.179299999999998</v>
@@ -1398,22 +1393,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>254</v>
+        <v>71</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="E6" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F6" t="s">
-        <v>179</v>
+        <v>78</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>235</v>
       </c>
       <c r="H6">
         <v>38.241943999999997</v>
@@ -1427,22 +1422,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>255</v>
+        <v>72</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="F7" t="s">
-        <v>185</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>89</v>
+        <v>235</v>
       </c>
       <c r="H7">
         <v>42.25</v>
@@ -1456,22 +1451,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>256</v>
+        <v>73</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="F8" t="s">
-        <v>183</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>236</v>
       </c>
       <c r="H8">
         <v>34.928333000000002</v>
@@ -1485,22 +1480,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>239</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="D9" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="F9" t="s">
-        <v>192</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H9">
         <v>42.393611</v>
@@ -1514,22 +1509,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>240</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="D10" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
-        <v>188</v>
+        <v>82</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>237</v>
       </c>
       <c r="H10">
         <v>37.321666999999998</v>
@@ -1543,22 +1538,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>241</v>
+        <v>58</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F11" t="s">
-        <v>197</v>
+        <v>83</v>
       </c>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>237</v>
       </c>
       <c r="H11">
         <v>37.35</v>
@@ -1572,22 +1567,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>242</v>
+        <v>59</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>203</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>204</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>205</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>236</v>
       </c>
       <c r="H12">
         <v>35.614919</v>
@@ -1601,22 +1596,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>243</v>
+        <v>60</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="D13" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="E13" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
-        <v>195</v>
+        <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>237</v>
       </c>
       <c r="H13">
         <v>38.286667000000001</v>
@@ -1630,22 +1625,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>244</v>
+        <v>61</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>206</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>207</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="F14" t="s">
-        <v>208</v>
+        <v>86</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>237</v>
       </c>
       <c r="H14">
         <v>42.713332999999999</v>
@@ -1659,22 +1654,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>245</v>
+        <v>62</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>209</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>210</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>211</v>
+        <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>212</v>
+        <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H15">
         <v>43.116388999999998</v>
@@ -1688,22 +1683,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>246</v>
+        <v>63</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>198</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>153</v>
       </c>
       <c r="E16" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="F16" t="s">
-        <v>201</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H16">
         <v>39.870832999999998</v>
@@ -1717,22 +1712,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>99</v>
+        <v>244</v>
       </c>
       <c r="D17" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>246</v>
       </c>
       <c r="F17" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="G17" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H17">
         <v>37.531388999999997</v>
@@ -1746,22 +1741,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>232</v>
+        <v>49</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>213</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>214</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>204</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G18" t="s">
-        <v>96</v>
+        <v>242</v>
       </c>
       <c r="H18">
         <v>35.766666999999998</v>
@@ -1775,22 +1770,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>233</v>
+        <v>50</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>103</v>
+        <v>247</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>248</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="G19" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H19">
         <v>38.894167000000003</v>
@@ -1804,22 +1799,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>234</v>
+        <v>51</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>107</v>
+        <v>250</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>251</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="F20" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="G20" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H20">
         <v>40.298889000000003</v>
@@ -1833,22 +1828,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>235</v>
+        <v>52</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="D21" t="s">
-        <v>115</v>
+        <v>256</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="F21" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="G21" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H21">
         <v>41.54</v>
@@ -1862,22 +1857,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>236</v>
+        <v>53</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>110</v>
+        <v>252</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>253</v>
       </c>
       <c r="E22" t="s">
-        <v>112</v>
+        <v>254</v>
       </c>
       <c r="F22" t="s">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H22">
         <v>44.814444000000002</v>
@@ -1888,25 +1883,25 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>93</v>
+        <v>239</v>
       </c>
       <c r="B23" t="s">
-        <v>237</v>
+        <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H23">
         <v>40.839244000000001</v>
@@ -1920,22 +1915,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>238</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H24">
         <v>39.149721999999997</v>
@@ -1949,22 +1944,22 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>40</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="F25" t="s">
-        <v>125</v>
+        <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H25">
         <v>41.185277999999997</v>
@@ -1978,22 +1973,22 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>224</v>
+        <v>41</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="D26" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="E26" t="s">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="F26" t="s">
-        <v>134</v>
+        <v>4</v>
       </c>
       <c r="G26" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H26">
         <v>40.738889</v>
@@ -2007,22 +2002,22 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>225</v>
+        <v>42</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
+        <v>5</v>
       </c>
       <c r="G27" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H27">
         <v>39.1</v>
@@ -2036,22 +2031,22 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>226</v>
+        <v>43</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="E28" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="F28" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H28">
         <v>38.158056000000002</v>
@@ -2065,22 +2060,22 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>227</v>
+        <v>44</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="F29" t="s">
-        <v>137</v>
+        <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H29">
         <v>40.707777999999998</v>
@@ -2094,22 +2089,22 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>228</v>
+        <v>45</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>254</v>
       </c>
       <c r="F30" t="s">
-        <v>140</v>
+        <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H30">
         <v>43.531666999999999</v>
@@ -2123,22 +2118,22 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>229</v>
+        <v>46</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="E31" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="G31" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H31">
         <v>41.666666999999997</v>
@@ -2152,22 +2147,22 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>230</v>
+        <v>47</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="E32" t="s">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="F32" t="s">
-        <v>147</v>
+        <v>10</v>
       </c>
       <c r="G32" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H32">
         <v>41.783332999999999</v>
@@ -2181,22 +2176,22 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>231</v>
+        <v>48</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="D33" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="F33" t="s">
-        <v>151</v>
+        <v>11</v>
       </c>
       <c r="G33" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H33">
         <v>37.493611000000001</v>
@@ -2210,22 +2205,22 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>215</v>
+        <v>32</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="E34" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="F34" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H34">
         <v>33.749721999999998</v>
@@ -2239,22 +2234,22 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>33</v>
       </c>
       <c r="C35" s="4">
         <v>4897</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="E35" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="F35" t="s">
-        <v>157</v>
+        <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H35">
         <v>42.345832999999999</v>
@@ -2268,22 +2263,22 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>217</v>
+        <v>34</v>
       </c>
       <c r="C36" s="4">
         <v>1700</v>
       </c>
       <c r="D36" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="E36" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="F36" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="G36" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H36">
         <v>30.24</v>
@@ -2297,22 +2292,22 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>217</v>
       </c>
       <c r="C37" s="4">
         <v>3296</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>218</v>
       </c>
       <c r="E37" t="s">
-        <v>66</v>
+        <v>219</v>
       </c>
       <c r="F37" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H37">
         <v>33.888551</v>
@@ -2326,22 +2321,22 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>220</v>
       </c>
       <c r="C38" s="4">
         <v>3482</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>221</v>
       </c>
       <c r="E38" t="s">
-        <v>70</v>
+        <v>222</v>
       </c>
       <c r="F38" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H38">
         <v>41.245328999999998</v>
@@ -2355,22 +2350,22 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>218</v>
+        <v>35</v>
       </c>
       <c r="C39" s="4">
         <v>7579</v>
       </c>
       <c r="D39" t="s">
-        <v>74</v>
+        <v>224</v>
       </c>
       <c r="E39" t="s">
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="F39" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="G39" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H39">
         <v>32.030439000000001</v>
@@ -2384,22 +2379,22 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>219</v>
+        <v>36</v>
       </c>
       <c r="C40" s="4">
         <v>2593</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>215</v>
       </c>
       <c r="E40" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="F40" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G40" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H40">
         <v>41.631110999999997</v>
@@ -2413,22 +2408,22 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>220</v>
+        <v>37</v>
       </c>
       <c r="C41" s="4">
         <v>7468</v>
       </c>
       <c r="D41" t="s">
-        <v>72</v>
+        <v>223</v>
       </c>
       <c r="E41" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="F41" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="G41" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H41">
         <v>42.267192000000001</v>
@@ -2442,22 +2437,22 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>221</v>
+        <v>38</v>
       </c>
       <c r="C42" s="4">
         <v>15571</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>228</v>
       </c>
       <c r="E42" t="s">
-        <v>81</v>
+        <v>229</v>
       </c>
       <c r="F42" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="G42" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H42">
         <v>33.667777999999998</v>
@@ -2471,22 +2466,22 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>222</v>
+        <v>39</v>
       </c>
       <c r="C43" s="4">
         <v>15527</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>226</v>
       </c>
       <c r="E43" t="s">
-        <v>78</v>
+        <v>227</v>
       </c>
       <c r="F43" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="G43" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="H43">
         <v>41.303888999999998</v>
@@ -2500,22 +2495,22 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="C44" s="4">
         <v>21035</v>
       </c>
       <c r="D44" t="s">
-        <v>83</v>
+        <v>230</v>
       </c>
       <c r="E44" t="s">
-        <v>84</v>
+        <v>231</v>
       </c>
       <c r="F44" t="s">
-        <v>86</v>
+        <v>232</v>
       </c>
       <c r="G44" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="H44">
         <v>21.300132999999999</v>
@@ -2525,10 +2520,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2552,18 +2545,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="B2">
         <v>61.384999999999998</v>
@@ -2574,7 +2567,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
       <c r="B3">
         <v>32.798999999999999</v>
@@ -2585,7 +2578,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>162</v>
       </c>
       <c r="B4">
         <v>34.951300000000003</v>
@@ -2596,7 +2589,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="B5">
         <v>14.2417</v>
@@ -2607,7 +2600,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B6">
         <v>33.7712</v>
@@ -2618,7 +2611,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="B7">
         <v>36.17</v>
@@ -2629,7 +2622,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="B8">
         <v>39.064599999999999</v>
@@ -2640,7 +2633,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
       <c r="B9">
         <v>41.583399999999997</v>
@@ -2651,7 +2644,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="B10">
         <v>38.8964</v>
@@ -2662,7 +2655,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>169</v>
       </c>
       <c r="B11">
         <v>39.349800000000002</v>
@@ -2673,7 +2666,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="B12">
         <v>27.833300000000001</v>
@@ -2684,7 +2677,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>171</v>
       </c>
       <c r="B13">
         <v>32.986600000000003</v>
@@ -2695,7 +2688,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
       <c r="B14">
         <v>21.1098</v>
@@ -2706,7 +2699,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>173</v>
       </c>
       <c r="B15">
         <v>42.004600000000003</v>
@@ -2717,7 +2710,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>174</v>
       </c>
       <c r="B16">
         <v>44.239400000000003</v>
@@ -2728,7 +2721,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>175</v>
       </c>
       <c r="B17">
         <v>40.336300000000001</v>
@@ -2739,7 +2732,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>176</v>
       </c>
       <c r="B18">
         <v>39.864699999999999</v>
@@ -2750,7 +2743,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>177</v>
       </c>
       <c r="B19">
         <v>38.511099999999999</v>
@@ -2761,7 +2754,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>178</v>
       </c>
       <c r="B20">
         <v>37.668999999999997</v>
@@ -2772,7 +2765,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>179</v>
       </c>
       <c r="B21">
         <v>31.180099999999999</v>
@@ -2783,7 +2776,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="B22">
         <v>42.237299999999998</v>
@@ -2794,7 +2787,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>181</v>
       </c>
       <c r="B23">
         <v>39.072400000000002</v>
@@ -2805,7 +2798,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>182</v>
       </c>
       <c r="B24">
         <v>44.607399999999998</v>
@@ -2816,7 +2809,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="B25">
         <v>43.3504</v>
@@ -2827,7 +2820,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>184</v>
       </c>
       <c r="B26">
         <v>45.732599999999998</v>
@@ -2838,7 +2831,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>185</v>
       </c>
       <c r="B27">
         <v>38.462299999999999</v>
@@ -2849,7 +2842,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>186</v>
       </c>
       <c r="B28">
         <v>14.8058</v>
@@ -2860,7 +2853,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="B29">
         <v>32.767299999999999</v>
@@ -2871,7 +2864,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>188</v>
       </c>
       <c r="B30">
         <v>46.904800000000002</v>
@@ -2882,7 +2875,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>189</v>
       </c>
       <c r="B31">
         <v>35.641100000000002</v>
@@ -2893,7 +2886,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>190</v>
       </c>
       <c r="B32">
         <v>47.536200000000001</v>
@@ -2904,7 +2897,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="B33">
         <v>41.128900000000002</v>
@@ -2915,7 +2908,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>192</v>
       </c>
       <c r="B34">
         <v>43.410800000000002</v>
@@ -2926,7 +2919,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>193</v>
       </c>
       <c r="B35">
         <v>40.314</v>
@@ -2937,7 +2930,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>194</v>
       </c>
       <c r="B36">
         <v>34.837499999999999</v>
@@ -2948,7 +2941,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>195</v>
       </c>
       <c r="B37">
         <v>38.419899999999998</v>
@@ -2959,7 +2952,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>196</v>
       </c>
       <c r="B38">
         <v>42.149700000000003</v>
@@ -2970,7 +2963,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>197</v>
       </c>
       <c r="B39">
         <v>40.373600000000003</v>
@@ -2981,7 +2974,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>198</v>
       </c>
       <c r="B40">
         <v>35.537599999999998</v>
@@ -2992,7 +2985,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>199</v>
       </c>
       <c r="B41">
         <v>44.5672</v>
@@ -3003,7 +2996,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="B42">
         <v>40.577300000000001</v>
@@ -3014,7 +3007,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>201</v>
       </c>
       <c r="B43">
         <v>18.276599999999998</v>
@@ -3025,7 +3018,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>202</v>
       </c>
       <c r="B44">
         <v>41.677199999999999</v>
@@ -3036,7 +3029,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="B45">
         <v>33.819099999999999</v>
@@ -3047,7 +3040,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>204</v>
       </c>
       <c r="B46">
         <v>44.285299999999999</v>
@@ -3058,7 +3051,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>205</v>
       </c>
       <c r="B47">
         <v>35.744900000000001</v>
@@ -3069,7 +3062,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>206</v>
       </c>
       <c r="B48">
         <v>31.106000000000002</v>
@@ -3080,7 +3073,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>207</v>
       </c>
       <c r="B49">
         <v>40.113500000000002</v>
@@ -3091,7 +3084,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>208</v>
       </c>
       <c r="B50">
         <v>37.768000000000001</v>
@@ -3102,7 +3095,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>209</v>
       </c>
       <c r="B51">
         <v>18.0001</v>
@@ -3113,7 +3106,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="B52">
         <v>44.040700000000001</v>
@@ -3124,7 +3117,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>211</v>
       </c>
       <c r="B53">
         <v>47.3917</v>
@@ -3135,7 +3128,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
       <c r="B54">
         <v>44.256300000000003</v>
@@ -3146,7 +3139,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>213</v>
       </c>
       <c r="B55">
         <v>38.468000000000004</v>
@@ -3157,7 +3150,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>214</v>
       </c>
       <c r="B56">
         <v>42.747500000000002</v>
@@ -3167,7 +3160,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>